<commit_message>
Updated code for transfer Order
</commit_message>
<xml_diff>
--- a/SnowTests/src/test/resources/testdata/AutomationTest Data.xlsx
+++ b/SnowTests/src/test/resources/testdata/AutomationTest Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centurylink-my.sharepoint.com/personal/rajneesh_k_gautam_lumen_com/Documents/Documents/All data/CM3 Data/SNOW_STAFF/SnowTests/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="11_F25DC773A252ABDACC104860E9DC56905BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C081760B-8B11-440C-9883-588A0D53D11C}"/>
+  <xr:revisionPtr revIDLastSave="568" documentId="11_F25DC773A252ABDACC104860E9DC56905BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{983FC343-CD79-4C35-90EF-54225A242605}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UNI_Install" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="117">
   <si>
     <t>Attributes</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>MOVE UNI Order-changing designator value FLR -1 and RM-NID1 from FLR-5 and RM-WLAB for service-</t>
+  </si>
+  <si>
+    <t>29/KXGS/595200//MS</t>
   </si>
 </sst>
 </file>
@@ -1643,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B6B3B8-389C-42EC-A03C-296310B1F74B}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,6 +1675,9 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
       </c>
       <c r="C3" t="s">
         <v>75</v>
@@ -1998,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AFFD74-D2AD-4482-B11F-AD9C1AA27C25}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Code & Feature File
</commit_message>
<xml_diff>
--- a/SnowTests/src/test/resources/testdata/AutomationTest Data.xlsx
+++ b/SnowTests/src/test/resources/testdata/AutomationTest Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centurylink-my.sharepoint.com/personal/rajneesh_k_gautam_lumen_com/Documents/Documents/All data/CM3 Data/SNOW_STAFF/SnowTests/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="568" documentId="11_F25DC773A252ABDACC104860E9DC56905BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{983FC343-CD79-4C35-90EF-54225A242605}"/>
+  <xr:revisionPtr revIDLastSave="575" documentId="11_F25DC773A252ABDACC104860E9DC56905BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A8F29EF-A0F7-4382-A452-E55D1A5C8588}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UNI_Install" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="MOVE_Order" sheetId="16" r:id="rId16"/>
     <sheet name="TRANSFER_Order" sheetId="17" r:id="rId17"/>
     <sheet name="Reference_Order" sheetId="6" r:id="rId18"/>
+    <sheet name="ServiceCleanup" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="124">
   <si>
     <t>Attributes</t>
   </si>
@@ -393,6 +394,27 @@
   </si>
   <si>
     <t>29/KXGS/595200//MS</t>
+  </si>
+  <si>
+    <t>EVC/OVC End Point Cleanup</t>
+  </si>
+  <si>
+    <t>IdentifierId</t>
+  </si>
+  <si>
+    <t>CorrelationId</t>
+  </si>
+  <si>
+    <t>UNI Service Cleanup</t>
+  </si>
+  <si>
+    <t>UNI Service Id</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>CustomerNo</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B6B3B8-389C-42EC-A03C-296310B1F74B}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1823,6 +1845,60 @@
       </c>
       <c r="B9" t="s">
         <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679637E3-4144-4DFB-82B0-5CA288076457}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2443,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8239C-82E3-41A4-9A00-E6DB83002FCB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>